<commit_message>
Last bits making PSA work
</commit_message>
<xml_diff>
--- a/Data/Costs.xlsx
+++ b/Data/Costs.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cm1om\Documents\Research\Cancer\Bladder\Bladder_cancer_model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC625404-851D-4E9C-8ED9-7BB8115DAC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5705941-8776-4DFD-8FE1-51CE40A1575B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="diagnostic costs" sheetId="1" r:id="rId1"/>
+    <sheet name="state costs" sheetId="2" r:id="rId2"/>
+    <sheet name="screen costs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,8 +35,76 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Chloe</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{62DD8C59-909D-4FCD-9B31-5C8E1C2223BF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chloe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1 = Beta
+2 = Gamma
+3 = Lognormal
+4 = Uniform
+4 = Correlated Parameter sets from calibration
+6 = Constant</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{6A8DAE32-D486-4FED-953A-C5020CE5D0C8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chloe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1 = Beta
+2 = Gamma
+3 = Lognormal
+4 = Uniform
+4 = Correlated Parameter sets from calibration
+6 = Constant</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="212">
   <si>
     <t>https://bmjopen.bmj.com/content/bmjopen/3/6/e002861.full.pdf</t>
   </si>
@@ -295,6 +365,393 @@
   </si>
   <si>
     <t xml:space="preserve">Total diagnostic costs </t>
+  </si>
+  <si>
+    <t>Total Costs</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF2E2E2E"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t> &gt; z</t>
+    </r>
+  </si>
+  <si>
+    <t>95% CI</t>
+  </si>
+  <si>
+    <t>Tumor recurrence</t>
+  </si>
+  <si>
+    <t> Unknown</t>
+  </si>
+  <si>
+    <t>−1871.636 to 4906.082</t>
+  </si>
+  <si>
+    <t> Grade 1</t>
+  </si>
+  <si>
+    <t>402.1653 to 2032.711</t>
+  </si>
+  <si>
+    <t> Grade 2</t>
+  </si>
+  <si>
+    <t>919.5377 to 2432.564</t>
+  </si>
+  <si>
+    <t> Grade 3</t>
+  </si>
+  <si>
+    <t>2331.122 to 5582.212</t>
+  </si>
+  <si>
+    <t>Risk group, high risk</t>
+  </si>
+  <si>
+    <t>1357.397 to 2578.431</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t> 2</t>
+  </si>
+  <si>
+    <t>−921.3536</t>
+  </si>
+  <si>
+    <t>−3.66</t>
+  </si>
+  <si>
+    <t>−1414.686 to −428.0217</t>
+  </si>
+  <si>
+    <t> 3</t>
+  </si>
+  <si>
+    <t>−1514.189</t>
+  </si>
+  <si>
+    <t>−6.47</t>
+  </si>
+  <si>
+    <t>−1972.806 to −1055.571</t>
+  </si>
+  <si>
+    <t>Risk group &amp; year</t>
+  </si>
+  <si>
+    <t> High risk &amp; year 2</t>
+  </si>
+  <si>
+    <t>−1511.85</t>
+  </si>
+  <si>
+    <t>−4.40</t>
+  </si>
+  <si>
+    <t>−2185.702 to −837.997</t>
+  </si>
+  <si>
+    <t> High risk &amp; year 3</t>
+  </si>
+  <si>
+    <t>−1894.898</t>
+  </si>
+  <si>
+    <t>−5.92</t>
+  </si>
+  <si>
+    <t>−2522.036 to −1267.759</t>
+  </si>
+  <si>
+    <t>Progression</t>
+  </si>
+  <si>
+    <t>2662.332 to 8151.544</t>
+  </si>
+  <si>
+    <t>Progression history</t>
+  </si>
+  <si>
+    <t>687.7356 to 3850.54</t>
+  </si>
+  <si>
+    <t>TCC history</t>
+  </si>
+  <si>
+    <t>−87.80923 to 270.8796</t>
+  </si>
+  <si>
+    <t>Patient gender</t>
+  </si>
+  <si>
+    <t>−42.12716 to 366.9096</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>−67.09895</t>
+  </si>
+  <si>
+    <t>−0.46</t>
+  </si>
+  <si>
+    <t>−355.2838 to 221.0859</t>
+  </si>
+  <si>
+    <t>Celecoxib treatment</t>
+  </si>
+  <si>
+    <t>−103.1504</t>
+  </si>
+  <si>
+    <t>−1.14</t>
+  </si>
+  <si>
+    <t>−280.6405 to 74.33965</t>
+  </si>
+  <si>
+    <t>Toxicity</t>
+  </si>
+  <si>
+    <t> Mild condition</t>
+  </si>
+  <si>
+    <t>−150.2041 to 531.0055</t>
+  </si>
+  <si>
+    <t> Moderate condition</t>
+  </si>
+  <si>
+    <t>−417.415 to 760.885</t>
+  </si>
+  <si>
+    <t>Celecoxib treatment &amp; toxicity interaction</t>
+  </si>
+  <si>
+    <t> Interaction</t>
+  </si>
+  <si>
+    <t> 1 &amp; Mild condition</t>
+  </si>
+  <si>
+    <t>−321.6498 to 628.1292</t>
+  </si>
+  <si>
+    <t> 1 &amp; Moderate condition</t>
+  </si>
+  <si>
+    <t>−369.9651 to 1150.08</t>
+  </si>
+  <si>
+    <t>Age, y</t>
+  </si>
+  <si>
+    <t> 50-59</t>
+  </si>
+  <si>
+    <t>−343.0704 to 416.7831</t>
+  </si>
+  <si>
+    <t> 60-69</t>
+  </si>
+  <si>
+    <t>−284.9767 to 410.3913</t>
+  </si>
+  <si>
+    <t> 70-79</t>
+  </si>
+  <si>
+    <t>−78.92821</t>
+  </si>
+  <si>
+    <t>−0.43</t>
+  </si>
+  <si>
+    <t>−436.676 to 278.8195</t>
+  </si>
+  <si>
+    <t> &gt;80</t>
+  </si>
+  <si>
+    <t>−385.8824 to 503.9342</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t> Overweight</t>
+  </si>
+  <si>
+    <t>19.95362 to 395.4054</t>
+  </si>
+  <si>
+    <t> Obese</t>
+  </si>
+  <si>
+    <t>35.96402 to 480.1804</t>
+  </si>
+  <si>
+    <t> Morbidly obese</t>
+  </si>
+  <si>
+    <t>36.31178 to 2479.624</t>
+  </si>
+  <si>
+    <t>Smoking status</t>
+  </si>
+  <si>
+    <t> Previous</t>
+  </si>
+  <si>
+    <t>−57.20011</t>
+  </si>
+  <si>
+    <t>−0.59</t>
+  </si>
+  <si>
+    <t>−247.6996 to 133.2993</t>
+  </si>
+  <si>
+    <t> Current</t>
+  </si>
+  <si>
+    <t>−241.9663</t>
+  </si>
+  <si>
+    <t>−1.98</t>
+  </si>
+  <si>
+    <t>−481.8741 to −2.058529</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>1750.875 to 2946.718</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1558767319303775?via%3Dihub#appsec1</t>
+  </si>
+  <si>
+    <t> Previous smoke</t>
+  </si>
+  <si>
+    <t> Current smoke</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>stage 4</t>
+  </si>
+  <si>
+    <t>stage 3</t>
+  </si>
+  <si>
+    <t>stage 1</t>
+  </si>
+  <si>
+    <t>stage 2</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>Average costs for grade1/2</t>
+  </si>
+  <si>
+    <t>Y1,50,non-smoker, stage 1</t>
+  </si>
+  <si>
+    <t>Y1,50,non-smoker, stage 2</t>
+  </si>
+  <si>
+    <t>Y1,50,non-smoker, stage 3</t>
+  </si>
+  <si>
+    <t>Y1,50,non-smoker, stage 4</t>
+  </si>
+  <si>
+    <t>Y1,50,non-smoker, Lg</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>Y£</t>
+  </si>
+  <si>
+    <t>Cost of FIT invite</t>
+  </si>
+  <si>
+    <t>Cost_FIT_invite</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Additional cost of FIT performed</t>
+  </si>
+  <si>
+    <t>Cost_FIT_perform</t>
+  </si>
+  <si>
+    <t>Additional cost of FIT positive result</t>
+  </si>
+  <si>
+    <t>Cost_FIT_positive</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Distribution type</t>
+  </si>
+  <si>
+    <t>Distribution Number</t>
+  </si>
+  <si>
+    <t>Distribution parameters</t>
+  </si>
+  <si>
+    <t>Southern Hub screening costings model inflated to 2017</t>
+  </si>
+  <si>
+    <t>Cost of one invite</t>
+  </si>
+  <si>
+    <t>Additional cost of one test  performed</t>
+  </si>
+  <si>
+    <t>Additional cost of a positive result</t>
+  </si>
+  <si>
+    <t>Costs of dipstick</t>
   </si>
 </sst>
 </file>
@@ -313,7 +770,7 @@
     <numFmt numFmtId="168" formatCode="###,###,###"/>
     <numFmt numFmtId="169" formatCode="0.00000000000000%"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,8 +962,50 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF2E2E2E"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF2E2E2E"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2E2E2E"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -636,8 +1135,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -885,6 +1390,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFEBEBEB"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -949,7 +1474,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1005,11 +1530,58 @@
     <xf numFmtId="8" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="58">
     <cellStyle name="20% - Accent1 2" xfId="6" xr:uid="{4847A1CF-D309-4339-8E03-3C8A39A5569D}"/>
@@ -1349,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,18 +1971,18 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39" t="s">
+      <c r="C4" s="41"/>
+      <c r="D4" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39" t="s">
+      <c r="E4" s="41"/>
+      <c r="F4" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="39"/>
+      <c r="G4" s="41"/>
       <c r="K4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1543,11 +2115,11 @@
         <v>0.50495049504950495</v>
       </c>
       <c r="F8" s="17">
-        <f>$A8*D8*$L$32</f>
+        <f t="shared" ref="F8:G12" si="0">$A8*D8*$L$32</f>
         <v>21.961923808231827</v>
       </c>
       <c r="G8" s="17">
-        <f>$A8*E8*$L$32</f>
+        <f t="shared" si="0"/>
         <v>18.644531728040374</v>
       </c>
       <c r="H8" s="12"/>
@@ -1579,19 +2151,19 @@
         <v>46</v>
       </c>
       <c r="D9" s="35">
-        <f t="shared" ref="D9:D12" si="0">B9/B$6</f>
+        <f t="shared" ref="D9:D12" si="1">B9/B$6</f>
         <v>0.29368029739776952</v>
       </c>
       <c r="E9" s="35">
-        <f t="shared" ref="E9:E11" si="1">C9/C$6</f>
+        <f t="shared" ref="E9:E11" si="2">C9/C$6</f>
         <v>0.22772277227722773</v>
       </c>
       <c r="F9" s="17">
-        <f>$A9*D9*$L$32</f>
+        <f t="shared" si="0"/>
         <v>21.687399760628928</v>
       </c>
       <c r="G9" s="17">
-        <f>$A9*E9*$L$32</f>
+        <f t="shared" si="0"/>
         <v>16.816636460585435</v>
       </c>
       <c r="H9" s="12"/>
@@ -1623,19 +2195,19 @@
         <v>23</v>
       </c>
       <c r="D10" s="35">
+        <f t="shared" si="1"/>
+        <v>7.434944237918216E-2</v>
+      </c>
+      <c r="E10" s="35">
+        <f t="shared" si="2"/>
+        <v>0.11386138613861387</v>
+      </c>
+      <c r="F10" s="17">
         <f t="shared" si="0"/>
-        <v>7.434944237918216E-2</v>
-      </c>
-      <c r="E10" s="35">
-        <f t="shared" si="1"/>
-        <v>0.11386138613861387</v>
-      </c>
-      <c r="F10" s="17">
-        <f>$A10*D10*$L$32</f>
         <v>8.2357214280869346</v>
       </c>
       <c r="G10" s="17">
-        <f>$A10*E10*$L$32</f>
+        <f t="shared" si="0"/>
         <v>12.612477345439077</v>
       </c>
       <c r="H10" s="12"/>
@@ -1664,19 +2236,19 @@
         <v>11</v>
       </c>
       <c r="D11" s="35">
+        <f t="shared" si="1"/>
+        <v>1.4869888475836431E-2</v>
+      </c>
+      <c r="E11" s="35">
+        <f t="shared" si="2"/>
+        <v>5.4455445544554455E-2</v>
+      </c>
+      <c r="F11" s="17">
         <f t="shared" si="0"/>
-        <v>1.4869888475836431E-2</v>
-      </c>
-      <c r="E11" s="35">
-        <f t="shared" si="1"/>
-        <v>5.4455445544554455E-2</v>
-      </c>
-      <c r="F11" s="17">
-        <f>$A11*D11*$L$32</f>
         <v>2.1961923808231827</v>
       </c>
       <c r="G11" s="17">
-        <f>$A11*E11*$L$32</f>
+        <f t="shared" si="0"/>
         <v>8.0427391768017298</v>
       </c>
       <c r="H11" s="12"/>
@@ -1705,7 +2277,7 @@
         <v>20</v>
       </c>
       <c r="D12" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2304832713754646E-2</v>
       </c>
       <c r="E12" s="35">
@@ -1713,11 +2285,11 @@
         <v>9.9009900990099015E-2</v>
       </c>
       <c r="F12" s="17">
-        <f>$A12*D12*$L$32</f>
+        <f t="shared" si="0"/>
         <v>4.1178607140434673</v>
       </c>
       <c r="G12" s="17">
-        <f>$A12*E12*$L$32</f>
+        <f t="shared" si="0"/>
         <v>18.278952674549384</v>
       </c>
       <c r="H12" s="12"/>
@@ -1777,11 +2349,11 @@
         <v>143</v>
       </c>
       <c r="D14" s="35">
-        <f t="shared" ref="D14:D21" si="2">B14/B$6</f>
+        <f t="shared" ref="D14:D21" si="3">B14/B$6</f>
         <v>0.73234200743494426</v>
       </c>
       <c r="E14" s="35">
-        <f t="shared" ref="E14:E21" si="3">C14/C$6</f>
+        <f t="shared" ref="E14:E21" si="4">C14/C$6</f>
         <v>0.70792079207920788</v>
       </c>
       <c r="F14" s="36">
@@ -1822,11 +2394,11 @@
         <v>59</v>
       </c>
       <c r="D15" s="35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.26765799256505574</v>
       </c>
       <c r="E15" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.29207920792079206</v>
       </c>
       <c r="F15" s="12"/>
@@ -1881,11 +2453,11 @@
         <v>36</v>
       </c>
       <c r="D17" s="35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.24907063197026E-2</v>
       </c>
       <c r="E17" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.17821782178217821</v>
       </c>
       <c r="F17" s="36">
@@ -1918,11 +2490,11 @@
         <v>166</v>
       </c>
       <c r="D18" s="35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.92750929368029744</v>
       </c>
       <c r="E18" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.82178217821782173</v>
       </c>
       <c r="F18" s="12"/>
@@ -1975,11 +2547,11 @@
         <v>47</v>
       </c>
       <c r="D20" s="35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.38475836431226768</v>
       </c>
       <c r="E20" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.23267326732673269</v>
       </c>
       <c r="F20" s="36">
@@ -2010,11 +2582,11 @@
         <v>155</v>
       </c>
       <c r="D21" s="35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.61524163568773238</v>
       </c>
       <c r="E21" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.76732673267326734</v>
       </c>
       <c r="F21" s="12"/>
@@ -2467,7 +3039,7 @@
       <c r="A47">
         <v>2015</v>
       </c>
-      <c r="B47" s="41">
+      <c r="B47" s="40">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="C47" s="19">
@@ -2478,7 +3050,7 @@
       <c r="A48">
         <v>2016</v>
       </c>
-      <c r="B48" s="41">
+      <c r="B48" s="40">
         <v>2.4E-2</v>
       </c>
       <c r="C48">
@@ -2489,7 +3061,7 @@
       <c r="A49">
         <v>2017</v>
       </c>
-      <c r="B49" s="41">
+      <c r="B49" s="40">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="C49">
@@ -2500,7 +3072,7 @@
       <c r="A50">
         <v>2018</v>
       </c>
-      <c r="B50" s="41">
+      <c r="B50" s="40">
         <v>2.3E-2</v>
       </c>
       <c r="C50">
@@ -2511,7 +3083,7 @@
       <c r="A51">
         <v>2019</v>
       </c>
-      <c r="B51" s="41">
+      <c r="B51" s="40">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="C51">
@@ -2522,7 +3094,7 @@
       <c r="A52">
         <v>2020</v>
       </c>
-      <c r="B52" s="41">
+      <c r="B52" s="40">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="C52">
@@ -2534,19 +3106,19 @@
       <c r="A53">
         <v>2021</v>
       </c>
-      <c r="B53" s="41">
+      <c r="B53" s="40">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="C53">
         <v>111.551</v>
       </c>
-      <c r="F53" s="40"/>
+      <c r="F53" s="39"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2022</v>
       </c>
-      <c r="B54" s="41">
+      <c r="B54" s="40">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="C54">
@@ -2625,4 +3197,1243 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33867B3-A7A4-41B0-880B-2F0FE2EB18BE}">
+  <dimension ref="A1:S40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="O3" t="s">
+        <v>192</v>
+      </c>
+      <c r="P3" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>189</v>
+      </c>
+      <c r="R3" t="s">
+        <v>190</v>
+      </c>
+      <c r="S3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="43">
+        <v>1517.223</v>
+      </c>
+      <c r="C4" s="43">
+        <v>1729.0409999999999</v>
+      </c>
+      <c r="D4" s="43">
+        <v>0.88</v>
+      </c>
+      <c r="E4" s="43">
+        <v>0.38</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="49"/>
+      <c r="H4" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="J4" s="51">
+        <v>2348.7959999999998</v>
+      </c>
+      <c r="K4" s="51">
+        <v>305.06760000000003</v>
+      </c>
+      <c r="L4" s="51">
+        <v>7.7</v>
+      </c>
+      <c r="N4" s="49" t="s">
+        <v>193</v>
+      </c>
+      <c r="O4">
+        <f>J4+J8+J16</f>
+        <v>3603.0903399999997</v>
+      </c>
+      <c r="P4">
+        <f>J4+J8+J19</f>
+        <v>3832.3968399999994</v>
+      </c>
+      <c r="Q4">
+        <f>J4+J8+J17</f>
+        <v>4061.7033399999996</v>
+      </c>
+      <c r="R4">
+        <f>J4+J8+J18</f>
+        <v>6342.31934</v>
+      </c>
+      <c r="S4">
+        <f>J4+J8+J15</f>
+        <v>7792.5903399999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="43">
+        <v>1217.4380000000001</v>
+      </c>
+      <c r="C5" s="43">
+        <v>415.9633</v>
+      </c>
+      <c r="D5" s="43">
+        <v>2.93</v>
+      </c>
+      <c r="E5" s="43">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="49"/>
+      <c r="H5" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="J5" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="K5" s="53">
+        <v>97.19538</v>
+      </c>
+      <c r="L5" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="N5" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="O5">
+        <f>J4+J8+J16+J13</f>
+        <v>2681.7367399999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="43">
+        <v>1676.0509999999999</v>
+      </c>
+      <c r="C6" s="43">
+        <v>385.98309999999998</v>
+      </c>
+      <c r="D6" s="43">
+        <v>4.34</v>
+      </c>
+      <c r="E6" s="43">
+        <v>0</v>
+      </c>
+      <c r="F6" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="49"/>
+      <c r="H6" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="J6" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="K6" s="53">
+        <v>122.4042</v>
+      </c>
+      <c r="L6" s="53" t="s">
+        <v>174</v>
+      </c>
+      <c r="N6" s="53" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="43">
+        <v>3956.6669999999999</v>
+      </c>
+      <c r="C7" s="43">
+        <v>829.37509999999997</v>
+      </c>
+      <c r="D7" s="43">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="E7" s="43">
+        <v>0</v>
+      </c>
+      <c r="F7" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="49"/>
+      <c r="H7" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="N7" s="49"/>
+    </row>
+    <row r="8" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="43">
+        <v>1967.914</v>
+      </c>
+      <c r="C8" s="43">
+        <v>311.49400000000003</v>
+      </c>
+      <c r="D8" s="43">
+        <v>6.32</v>
+      </c>
+      <c r="E8" s="43">
+        <v>0</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="49"/>
+      <c r="H8" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="J8" s="53">
+        <v>36.856340000000003</v>
+      </c>
+      <c r="K8" s="53">
+        <v>193.84370000000001</v>
+      </c>
+      <c r="L8" s="53">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="J9" s="53">
+        <v>62.707299999999996</v>
+      </c>
+      <c r="K9" s="53">
+        <v>177.3931</v>
+      </c>
+      <c r="L9" s="53">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="43">
+        <v>251.7046</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="43">
+        <v>0</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="49"/>
+      <c r="H10" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="J10" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="K10" s="53">
+        <v>182.52770000000001</v>
+      </c>
+      <c r="L10" s="53" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="43">
+        <v>233.99279999999999</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="43">
+        <v>0</v>
+      </c>
+      <c r="F11" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" s="49"/>
+      <c r="H11" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="J11" s="53">
+        <v>59.025919999999999</v>
+      </c>
+      <c r="K11" s="53">
+        <v>226.9982</v>
+      </c>
+      <c r="L11" s="53">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
+    </row>
+    <row r="13" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="43">
+        <v>343.80869999999999</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" s="43">
+        <v>0</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="49"/>
+      <c r="H13" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="J13" s="53">
+        <v>-921.35360000000003</v>
+      </c>
+      <c r="K13" s="53">
+        <v>251.7046</v>
+      </c>
+      <c r="L13" s="53" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="43">
+        <v>319.97449999999998</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="43">
+        <v>0</v>
+      </c>
+      <c r="F14" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="G14" s="49"/>
+      <c r="H14" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="J14" s="53">
+        <v>-1514.1890000000001</v>
+      </c>
+      <c r="K14" s="53">
+        <v>233.99279999999999</v>
+      </c>
+      <c r="L14" s="53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="43">
+        <v>5406.9380000000001</v>
+      </c>
+      <c r="C15" s="43">
+        <v>1400.335</v>
+      </c>
+      <c r="D15" s="43">
+        <v>3.86</v>
+      </c>
+      <c r="E15" s="43">
+        <v>0</v>
+      </c>
+      <c r="F15" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="H15" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="I15" s="49" t="s">
+        <v>182</v>
+      </c>
+      <c r="J15" s="53">
+        <v>5406.9380000000001</v>
+      </c>
+      <c r="K15" s="53">
+        <v>1400.335</v>
+      </c>
+      <c r="L15" s="53">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="43">
+        <v>2269.1379999999999</v>
+      </c>
+      <c r="C16" s="43">
+        <v>806.8528</v>
+      </c>
+      <c r="D16" s="43">
+        <v>2.81</v>
+      </c>
+      <c r="E16" s="43">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F16" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="H16" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="I16" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="J16" s="53">
+        <v>1217.4380000000001</v>
+      </c>
+      <c r="K16" s="53">
+        <v>415.9633</v>
+      </c>
+      <c r="L16" s="53">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="43">
+        <v>91.535179999999997</v>
+      </c>
+      <c r="C17" s="43">
+        <v>91.503929999999997</v>
+      </c>
+      <c r="D17" s="43">
+        <v>1</v>
+      </c>
+      <c r="E17" s="43">
+        <v>0.317</v>
+      </c>
+      <c r="F17" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="H17" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" s="49" t="s">
+        <v>185</v>
+      </c>
+      <c r="J17" s="53">
+        <v>1676.0509999999999</v>
+      </c>
+      <c r="K17" s="53">
+        <v>385.98309999999998</v>
+      </c>
+      <c r="L17" s="53">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="43">
+        <v>162.3912</v>
+      </c>
+      <c r="C18" s="43">
+        <v>104.348</v>
+      </c>
+      <c r="D18" s="43">
+        <v>1.56</v>
+      </c>
+      <c r="E18" s="43">
+        <v>0.12</v>
+      </c>
+      <c r="F18" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="H18" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="I18" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="J18" s="53">
+        <v>3956.6669999999999</v>
+      </c>
+      <c r="K18" s="53">
+        <v>829.37509999999997</v>
+      </c>
+      <c r="L18" s="53">
+        <v>4.7699999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="43">
+        <v>147.03579999999999</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="43">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="F19" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="H19" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="I19" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="J19" s="49">
+        <f>AVERAGE(J16:J17)</f>
+        <v>1446.7445</v>
+      </c>
+      <c r="K19" s="49">
+        <f>AVERAGE(K16:K17)</f>
+        <v>400.97320000000002</v>
+      </c>
+      <c r="L19" s="49">
+        <f>AVERAGE(L16:L17)</f>
+        <v>3.6349999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" s="43">
+        <v>90.557829999999996</v>
+      </c>
+      <c r="D20" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="E20" s="43">
+        <v>0.255</v>
+      </c>
+      <c r="F20" s="43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+    </row>
+    <row r="22" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="43">
+        <v>190.4007</v>
+      </c>
+      <c r="C22" s="43">
+        <v>173.78120000000001</v>
+      </c>
+      <c r="D22" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E22" s="43">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="43">
+        <v>171.73500000000001</v>
+      </c>
+      <c r="C23" s="43">
+        <v>300.59230000000002</v>
+      </c>
+      <c r="D23" s="43">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E23" s="43">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="F23" s="43" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+    </row>
+    <row r="25" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+    </row>
+    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" s="43">
+        <v>153.2397</v>
+      </c>
+      <c r="C26" s="43">
+        <v>242.29499999999999</v>
+      </c>
+      <c r="D26" s="43">
+        <v>0.63</v>
+      </c>
+      <c r="E26" s="43">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="43">
+        <v>390.0575</v>
+      </c>
+      <c r="C27" s="43">
+        <v>387.77379999999999</v>
+      </c>
+      <c r="D27" s="43">
+        <v>1.01</v>
+      </c>
+      <c r="E27" s="43">
+        <v>0.314</v>
+      </c>
+      <c r="F27" s="43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+    </row>
+    <row r="29" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" s="43">
+        <v>36.856340000000003</v>
+      </c>
+      <c r="C29" s="43">
+        <v>193.84370000000001</v>
+      </c>
+      <c r="D29" s="43">
+        <v>0.19</v>
+      </c>
+      <c r="E29" s="43">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="F29" s="43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" s="43">
+        <v>62.707299999999996</v>
+      </c>
+      <c r="C30" s="43">
+        <v>177.3931</v>
+      </c>
+      <c r="D30" s="43">
+        <v>0.35</v>
+      </c>
+      <c r="E30" s="43">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="F30" s="43" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" s="43">
+        <v>182.52770000000001</v>
+      </c>
+      <c r="D31" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" s="43">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="F31" s="43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32" s="43">
+        <v>59.025919999999999</v>
+      </c>
+      <c r="C32" s="43">
+        <v>226.9982</v>
+      </c>
+      <c r="D32" s="43">
+        <v>0.26</v>
+      </c>
+      <c r="E32" s="43">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="F32" s="43" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+    </row>
+    <row r="34" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="B34" s="43">
+        <v>207.67949999999999</v>
+      </c>
+      <c r="C34" s="43">
+        <v>95.780289999999994</v>
+      </c>
+      <c r="D34" s="43">
+        <v>2.17</v>
+      </c>
+      <c r="E34" s="43">
+        <v>0.03</v>
+      </c>
+      <c r="F34" s="43" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="43">
+        <v>258.07220000000001</v>
+      </c>
+      <c r="C35" s="43">
+        <v>113.32259999999999</v>
+      </c>
+      <c r="D35" s="43">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="E35" s="43">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F35" s="43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="B36" s="43">
+        <v>1257.9680000000001</v>
+      </c>
+      <c r="C36" s="43">
+        <v>623.30529999999999</v>
+      </c>
+      <c r="D36" s="43">
+        <v>2.02</v>
+      </c>
+      <c r="E36" s="43">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F36" s="43" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="B37" s="43"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+    </row>
+    <row r="38" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" s="43">
+        <v>97.19538</v>
+      </c>
+      <c r="D38" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="E38" s="43">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="F38" s="43" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" s="43">
+        <v>122.4042</v>
+      </c>
+      <c r="D39" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="E39" s="43">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F39" s="43" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="B40" s="46">
+        <v>2348.7959999999998</v>
+      </c>
+      <c r="C40" s="46">
+        <v>305.06760000000003</v>
+      </c>
+      <c r="D40" s="46">
+        <v>7.7</v>
+      </c>
+      <c r="E40" s="46">
+        <v>0</v>
+      </c>
+      <c r="F40" s="46" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE0144D-358F-44D8-95C5-63A01C199E30}">
+  <dimension ref="B1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" hidden="1" customWidth="1"/>
+    <col min="5" max="8" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="39" x14ac:dyDescent="0.25">
+      <c r="D1" s="55" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="55" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" s="56"/>
+      <c r="I1" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="57"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2">
+        <v>7.4516567327989689</v>
+      </c>
+      <c r="E2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:H4" si="0">D2/G2</f>
+        <v>7.4516567327989683E-2</v>
+      </c>
+      <c r="I2">
+        <v>6.7064910595190703</v>
+      </c>
+      <c r="J2">
+        <v>8.1968224060788675</v>
+      </c>
+      <c r="K2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3">
+        <v>1.0856698902187309</v>
+      </c>
+      <c r="E3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>1.0856698902187309E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.97710290119685794</v>
+      </c>
+      <c r="J3">
+        <v>1.1942368792406022</v>
+      </c>
+      <c r="K3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4">
+        <v>10.230186979795642</v>
+      </c>
+      <c r="E4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0.10230186979795641</v>
+      </c>
+      <c r="I4">
+        <v>9.2071682818160756</v>
+      </c>
+      <c r="J4">
+        <v>11.253205677775204</v>
+      </c>
+      <c r="K4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="39" x14ac:dyDescent="0.25">
+      <c r="B7" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>203</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>205</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" s="56"/>
+      <c r="I7" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="57"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8">
+        <f>D2+D2*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <v>8.5726758771672245</v>
+      </c>
+      <c r="E8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <f>D8/G8</f>
+        <v>8.572675877167224E-2</v>
+      </c>
+      <c r="I8">
+        <f>I2+I2*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <v>7.7154082894505009</v>
+      </c>
+      <c r="J8">
+        <f>J2+J2*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <v>9.4299434648839497</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D9">
+        <f>D3+D3*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <v>1.2489968891721883</v>
+      </c>
+      <c r="E9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <f>D9/G9</f>
+        <v>1.2489968891721883E-2</v>
+      </c>
+      <c r="I9">
+        <f>I3+I3*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <v>1.1240972002549696</v>
+      </c>
+      <c r="J9">
+        <f>J3+J3*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <v>1.373896578089405</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D10">
+        <f>D4+D4*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <v>11.769205196286959</v>
+      </c>
+      <c r="E10" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+      <c r="H10">
+        <f>D10/G10</f>
+        <v>0.1176920519628696</v>
+      </c>
+      <c r="I10">
+        <f>I4+I4*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <v>10.592284676658261</v>
+      </c>
+      <c r="J10">
+        <f>J4+J4*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <v>12.946125715915652</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Assigning health states code. Run pop as a multi-age cohort
</commit_message>
<xml_diff>
--- a/Data/Costs.xlsx
+++ b/Data/Costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cm1om\Documents\Research\Cancer\Bladder\Bladder_cancer_model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5705941-8776-4DFD-8FE1-51CE40A1575B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25E8444-5D39-4D68-9CA8-3528D31AFEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="diagnostic costs" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="214">
   <si>
     <t>https://bmjopen.bmj.com/content/bmjopen/3/6/e002861.full.pdf</t>
   </si>
@@ -253,9 +253,6 @@
     <t>cytology</t>
   </si>
   <si>
-    <t>Mowatt</t>
-  </si>
-  <si>
     <t>Symptomatic patient diagnosis</t>
   </si>
   <si>
@@ -353,9 +350,6 @@
   </si>
   <si>
     <t>Clinical oncology service</t>
-  </si>
-  <si>
-    <t>Screen-detected</t>
   </si>
   <si>
     <t>Percentage change</t>
@@ -752,6 +746,18 @@
   </si>
   <si>
     <t>Costs of dipstick</t>
+  </si>
+  <si>
+    <t>DAPS01</t>
+  </si>
+  <si>
+    <t>Cytology</t>
+  </si>
+  <si>
+    <t>Screen-positive</t>
+  </si>
+  <si>
+    <t>Screen-st1_positive</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1410,6 +1416,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1474,7 +1495,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1532,9 +1553,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1575,13 +1593,19 @@
     <xf numFmtId="0" fontId="5" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="5" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="58">
     <cellStyle name="20% - Accent1 2" xfId="6" xr:uid="{4847A1CF-D309-4339-8E03-3C8A39A5569D}"/>
@@ -1919,10 +1943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,20 +1964,20 @@
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M1" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M2" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1967,22 +1991,22 @@
         <v>22</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41" t="s">
+      <c r="C4" s="56"/>
+      <c r="D4" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="41"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="56"/>
       <c r="K4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1996,7 +2020,7 @@
         <v>358.35777993029501</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
       <c r="B5" s="33" t="s">
         <v>2</v>
@@ -2017,10 +2041,13 @@
         <v>4</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I5" s="34" t="s">
-        <v>83</v>
+        <v>212</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>213</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>13</v>
@@ -2030,7 +2057,7 @@
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>3</v>
       </c>
@@ -2052,6 +2079,7 @@
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
       <c r="K6" s="1" t="s">
         <v>14</v>
       </c>
@@ -2068,7 +2096,7 @@
         <v>24828.748786282544</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>5</v>
       </c>
@@ -2080,6 +2108,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
       <c r="K7" s="1" t="s">
         <v>16</v>
       </c>
@@ -2096,7 +2125,7 @@
         <v>17567.484424181195</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>1</v>
       </c>
@@ -2115,7 +2144,7 @@
         <v>0.50495049504950495</v>
       </c>
       <c r="F8" s="17">
-        <f t="shared" ref="F8:G12" si="0">$A8*D8*$L$32</f>
+        <f t="shared" ref="F8:G12" si="0">$A8*D8*$L$33</f>
         <v>21.961923808231827</v>
       </c>
       <c r="G8" s="17">
@@ -2124,6 +2153,7 @@
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
       <c r="K8" s="1" t="s">
         <v>17</v>
       </c>
@@ -2140,7 +2170,7 @@
         <v>10173.92823319062</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>2</v>
       </c>
@@ -2168,6 +2198,7 @@
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
       <c r="K9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2184,7 +2215,7 @@
         <v>5296.9190490700157</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>3</v>
       </c>
@@ -2212,6 +2243,7 @@
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
       <c r="L10" s="9" t="s">
         <v>31</v>
       </c>
@@ -2225,7 +2257,7 @@
         <v>11234.390715999065</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>4</v>
       </c>
@@ -2253,6 +2285,7 @@
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
       <c r="L11" s="9" t="s">
         <v>33</v>
       </c>
@@ -2266,7 +2299,7 @@
         <v>1493.0885035357869</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>5</v>
       </c>
@@ -2294,6 +2327,7 @@
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
       <c r="L12" s="9" t="s">
         <v>35</v>
       </c>
@@ -2307,10 +2341,7 @@
         <v>614.7279953162415</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
-        <v>6</v>
-      </c>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="35"/>
@@ -2325,6 +2356,7 @@
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
       <c r="L13" s="9" t="s">
         <v>37</v>
       </c>
@@ -2338,400 +2370,404 @@
         <v>3063.3545965175604</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="12">
-        <v>394</v>
-      </c>
-      <c r="C14" s="12">
-        <v>143</v>
-      </c>
-      <c r="D14" s="35">
-        <f t="shared" ref="D14:D21" si="3">B14/B$6</f>
-        <v>0.73234200743494426</v>
-      </c>
-      <c r="E14" s="35">
-        <f t="shared" ref="E14:E21" si="4">C14/C$6</f>
-        <v>0.70792079207920788</v>
-      </c>
-      <c r="F14" s="36">
-        <f>D14*$L$34</f>
-        <v>2.8256249296654277</v>
-      </c>
-      <c r="G14" s="36">
-        <f>E14*$L$34</f>
-        <v>2.7313995619801981</v>
-      </c>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
-      <c r="L14" s="9" t="s">
+      <c r="J14" s="12"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="11"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="12">
+        <v>394</v>
+      </c>
+      <c r="C15" s="12">
+        <v>143</v>
+      </c>
+      <c r="D15" s="35">
+        <f t="shared" ref="D15:D22" si="3">B15/B$6</f>
+        <v>0.73234200743494426</v>
+      </c>
+      <c r="E15" s="35">
+        <f t="shared" ref="E15:E22" si="4">C15/C$6</f>
+        <v>0.70792079207920788</v>
+      </c>
+      <c r="F15" s="36">
+        <f>D15*$L$35</f>
+        <v>4.3992762854160876</v>
+      </c>
+      <c r="G15" s="36">
+        <f>E15*$L$35</f>
+        <v>4.2525747819043227</v>
+      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="L15" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="10" t="s">
+      <c r="M15" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N15" s="7">
         <v>1583349</v>
       </c>
-      <c r="O14" s="11">
+      <c r="O15" s="11">
         <v>69.505783102777727</v>
       </c>
-      <c r="P14" s="19">
-        <f>(N14*O14+N15*O15)/SUM(N14:N15)</f>
+      <c r="P15" s="19">
+        <f>(N15*O15+N16*O16)/SUM(N15:N16)</f>
         <v>79.580236737963546</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B16" s="12">
         <v>144</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C16" s="12">
         <v>59</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D16" s="35">
         <f t="shared" si="3"/>
         <v>0.26765799256505574</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E16" s="35">
         <f t="shared" si="4"/>
         <v>0.29207920792079206</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="L15" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="N15" s="7">
-        <v>1370156</v>
-      </c>
-      <c r="O15" s="11">
-        <v>91.22225128872843</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
-      <c r="L16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="L16" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="M16" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="7">
+        <v>1370156</v>
+      </c>
+      <c r="O16" s="11">
+        <v>91.22225128872843</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="N16" s="12"/>
-      <c r="O16" s="6">
+      <c r="N17" s="12"/>
+      <c r="O17" s="6">
         <v>45</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B18" s="12">
         <v>39</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C18" s="12">
         <v>36</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D18" s="35">
         <f t="shared" si="3"/>
         <v>7.24907063197026E-2</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E18" s="35">
         <f t="shared" si="4"/>
         <v>0.17821782178217821</v>
       </c>
-      <c r="F17" s="36">
-        <f>D17*$L$35</f>
+      <c r="F18" s="36">
+        <f>D18*$L$37</f>
         <v>6.4547034791030358</v>
       </c>
-      <c r="G17" s="36">
-        <f>E17*$L$35</f>
+      <c r="G18" s="36">
+        <f>E18*$L$37</f>
         <v>15.868836885410966</v>
       </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="10" t="s">
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="N17" s="12"/>
-      <c r="O17" s="13">
+      <c r="N18" s="12"/>
+      <c r="O18" s="13">
         <v>303.36711779448615</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B19" s="12">
         <v>499</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C19" s="12">
         <v>166</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D19" s="35">
         <f t="shared" si="3"/>
         <v>0.92750929368029744</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E19" s="35">
         <f t="shared" si="4"/>
         <v>0.82178217821782173</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="L18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="M18" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="N18" s="12"/>
-      <c r="O18" s="13">
-        <v>684.7994910179641</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
-      <c r="L19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="L19" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="M19" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N19" s="12"/>
-      <c r="O19" s="12">
-        <v>92.37</v>
-      </c>
-      <c r="P19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="O19" s="13">
+        <v>684.7994910179641</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="L20" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="M20" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="N20" s="32">
+        <v>6</v>
+      </c>
+      <c r="O20" s="12"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B21" s="12">
         <v>207</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C21" s="12">
         <v>47</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D21" s="35">
         <f t="shared" si="3"/>
         <v>0.38475836431226768</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E21" s="35">
         <f t="shared" si="4"/>
         <v>0.23267326732673269</v>
       </c>
-      <c r="F20" s="36">
-        <f>D20*$L$33</f>
+      <c r="F21" s="36">
+        <f>D21*$L$34</f>
         <v>1.3158736059479554</v>
       </c>
-      <c r="G20" s="36">
-        <f>E20*$L$33</f>
+      <c r="G21" s="36">
+        <f>E21*$L$34</f>
         <v>0.79574257425742578</v>
       </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="L20" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="M20" s="18" t="s">
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="L21" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="M21" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B22" s="12">
         <v>331</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C22" s="12">
         <v>155</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D22" s="35">
         <f t="shared" si="3"/>
         <v>0.61524163568773238</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E22" s="35">
         <f t="shared" si="4"/>
         <v>0.76732673267326734</v>
       </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="M21" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="N21" s="29">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
-      <c r="L22" s="30" t="s">
-        <v>39</v>
-      </c>
+      <c r="J22" s="12"/>
       <c r="M22" s="28" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="N22" s="29">
-        <v>44</v>
-      </c>
-      <c r="O22">
-        <f>(N14*N22+N15*N24)/(N14+N15)</f>
-        <v>49.102993223305866</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>70</v>
-      </c>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
-      <c r="F23" s="37">
-        <f>SUM(F13:F20)</f>
-        <v>68.79530010653076</v>
-      </c>
-      <c r="G23" s="37">
-        <f>SUM(G13:G20)</f>
-        <v>93.791316407064599</v>
-      </c>
-      <c r="H23" s="37">
-        <f>F23*D6+G23*E6</f>
-        <v>75.61853698856838</v>
-      </c>
-      <c r="I23" s="17">
-        <f>SUM(F14:F20,L32)*D6+SUM(G14:G20,L32)*E6</f>
-        <v>49.921787708387654</v>
-      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
       <c r="L23" s="30" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="M23" s="28" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="N23" s="29">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="O23">
+        <f>(N15*N23+N16*N25)/(N15+N16)</f>
+        <v>49.102993223305866</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
-      <c r="H24" s="11">
-        <f>O4+O4*K32</f>
-        <v>400.96417872130121</v>
-      </c>
-      <c r="I24" s="38">
-        <f>H24</f>
-        <v>400.96417872130121</v>
-      </c>
+      <c r="F24" s="37">
+        <f>SUM(F13:F21)</f>
+        <v>70.368951462281416</v>
+      </c>
+      <c r="G24" s="37">
+        <f>SUM(G13:G21)</f>
+        <v>95.312491626988731</v>
+      </c>
+      <c r="H24" s="37">
+        <f>F24*D6+G24*E6</f>
+        <v>77.177863777512329</v>
+      </c>
+      <c r="I24" s="17">
+        <f>L33+L34+L35+L37</f>
+        <v>135.39242497873377</v>
+      </c>
+      <c r="J24" s="12"/>
       <c r="L24" s="30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M24" s="28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N24" s="29">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>70</v>
+      </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
+      <c r="H25" s="11">
+        <f>O4+O4*K33</f>
+        <v>400.96417872130121</v>
+      </c>
       <c r="I25" s="38"/>
+      <c r="J25" s="61">
+        <f>O4+O4*K33</f>
+        <v>400.96417872130121</v>
+      </c>
       <c r="L25" s="30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M25" s="28" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="N25" s="29">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>82</v>
-      </c>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="37">
-        <f>N26</f>
-        <v>134</v>
-      </c>
-      <c r="I26" s="38">
-        <f>H26</f>
-        <v>134</v>
-      </c>
-      <c r="M26" s="31" t="s">
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="12"/>
+      <c r="L26" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="M26" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="N26" s="29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
         <v>81</v>
-      </c>
-      <c r="N26" s="32">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -2740,112 +2776,104 @@
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="37">
-        <f>SUM(H23:H26)</f>
-        <v>610.5827157098696</v>
-      </c>
-      <c r="I27" s="37">
-        <f>SUM(I23:I26)</f>
-        <v>584.88596642968889</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+        <f>N27</f>
+        <v>134</v>
+      </c>
+      <c r="J27" s="38">
+        <f>H27</f>
+        <v>134</v>
+      </c>
+      <c r="M27" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="N27" s="32">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12" t="s">
+      <c r="H28" s="37">
+        <f>SUM(H24:H27)</f>
+        <v>612.14204249881357</v>
+      </c>
+      <c r="I28" s="37">
+        <f>SUM(I24:I27)</f>
+        <v>135.39242497873377</v>
+      </c>
+      <c r="J28" s="37">
+        <f>SUM(J24:J27)</f>
+        <v>534.96417872130121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="12"/>
+    </row>
+    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="12" t="s">
+      <c r="C32" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>1</v>
-      </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="L31" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="M31" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="N31" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="17">
-        <v>33</v>
-      </c>
-      <c r="C32" s="12">
-        <v>2020</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
-      <c r="J32" s="12">
-        <v>2022</v>
-      </c>
-      <c r="K32" s="12">
-        <f>(C54-C52)/C52</f>
-        <v>0.11889346674514417</v>
-      </c>
-      <c r="L32" s="23">
-        <f>B32+B32*K32</f>
-        <v>36.923484402589757</v>
-      </c>
-      <c r="M32" s="26">
-        <f>SUM(F13:F20)</f>
-        <v>68.79530010653076</v>
-      </c>
-      <c r="N32" s="27">
-        <f>SUM(G13:G20)</f>
-        <v>93.791316407064599</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J32" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="L32" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="M32" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="N32" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B33" s="17">
-        <v>3.42</v>
+        <v>33</v>
       </c>
       <c r="C33" s="12">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
@@ -2856,25 +2884,34 @@
         <v>2022</v>
       </c>
       <c r="K33" s="12">
-        <v>0</v>
+        <f>(C56-C54)/C54</f>
+        <v>0.11889346674514417</v>
       </c>
       <c r="L33" s="23">
-        <f>B33+B33*K33/100</f>
+        <f>B33+B33*K33</f>
+        <v>36.923484402589757</v>
+      </c>
+      <c r="M33" s="26">
+        <f>SUM(F13:F21)</f>
+        <v>70.368951462281416</v>
+      </c>
+      <c r="N33" s="27">
+        <f>SUM(G13:G21)</f>
+        <v>95.312491626988731</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="17">
         <v>3.42</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="17">
-        <v>3.85</v>
-      </c>
       <c r="C34" s="12">
-        <v>2015</v>
+        <v>2022</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
@@ -2885,23 +2922,21 @@
         <v>2022</v>
       </c>
       <c r="K34" s="12">
-        <f>(C54-C47)/C47</f>
-        <v>0.21664000000000003</v>
+        <v>0</v>
       </c>
       <c r="L34" s="23">
         <f>B34+B34*K34/100</f>
-        <v>3.8583406400000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="21">
-        <f>P14</f>
-        <v>79.580236737963546</v>
-      </c>
-      <c r="C35" s="20">
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="17">
+        <v>6</v>
+      </c>
+      <c r="C35" s="12">
         <v>2020</v>
       </c>
       <c r="D35" s="12"/>
@@ -2910,275 +2945,334 @@
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
-      <c r="J35" s="20">
+      <c r="J35" s="12">
         <v>2022</v>
       </c>
       <c r="K35" s="12">
-        <f>(C54-C52)*100/C52</f>
-        <v>11.889346674514417</v>
+        <f>K33</f>
+        <v>0.11889346674514417</v>
       </c>
       <c r="L35" s="23">
         <f>B35+B35*K35/100</f>
+        <v>6.0071336080047084</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="17">
+        <v>3.85</v>
+      </c>
+      <c r="C36" s="12">
+        <v>2015</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12">
+        <v>2022</v>
+      </c>
+      <c r="K36" s="12">
+        <f>(C56-C49)/C49</f>
+        <v>0.21664000000000003</v>
+      </c>
+      <c r="L36" s="23">
+        <f>B36+B36*K36/100</f>
+        <v>3.8583406400000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="21">
+        <f>P15</f>
+        <v>79.580236737963546</v>
+      </c>
+      <c r="C37" s="20">
+        <v>2020</v>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="20">
+        <v>2022</v>
+      </c>
+      <c r="K37" s="12">
+        <f>(C56-C54)*100/C54</f>
+        <v>11.889346674514417</v>
+      </c>
+      <c r="L37" s="23">
+        <f>B37+B37*K37/100</f>
         <v>89.041806968139312</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B38">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B40">
         <v>2016</v>
       </c>
-      <c r="C38">
+      <c r="C40">
         <v>2017</v>
       </c>
-      <c r="D38">
+      <c r="D40">
         <v>2018</v>
       </c>
-      <c r="E38">
+      <c r="E40">
         <v>2019</v>
       </c>
-      <c r="F38">
+      <c r="F40">
         <v>2020</v>
       </c>
-      <c r="G38">
+      <c r="G40">
         <v>2021</v>
       </c>
-      <c r="H38">
+      <c r="H40">
         <v>2022</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+    <row r="41" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="14">
+        <f>(B36+B36*0.35%)</f>
+        <v>3.8634750000000002</v>
+      </c>
+      <c r="C43" s="14">
+        <f>(B43*2.12%)+B43</f>
+        <v>3.94538067</v>
+      </c>
+      <c r="D43" s="14">
+        <f>(C43*1.16%)+C43</f>
+        <v>3.9911470857719999</v>
+      </c>
+      <c r="E43" s="14">
+        <f>(D43*2.31%)+D43</f>
+        <v>4.0833425834533328</v>
+      </c>
+      <c r="F43" s="14">
+        <f>(E43*B54)+E43</f>
+        <v>4.1282593518713195</v>
+      </c>
+      <c r="G43" s="14">
+        <f>F43+(F43*B55)</f>
+        <v>4.2190810576124882</v>
+      </c>
+      <c r="H43" s="14">
+        <f>G43+(G43*B56)</f>
+        <v>4.4215969483778874</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>50</v>
+      </c>
+      <c r="G44" s="14">
+        <f>B33+(B33*G$59)</f>
+        <v>33.725999999999999</v>
+      </c>
+      <c r="H44" s="14">
+        <f>G44+(G44*H$59)</f>
+        <v>35.344847999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="G45" s="14">
+        <f>B34+(B34*G$59)</f>
+        <v>3.4952399999999999</v>
+      </c>
+      <c r="H45" s="14">
+        <f>G45+(G45*H$59)</f>
+        <v>3.66301152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="14">
+        <f>B37+(B37*G$59)</f>
+        <v>81.331001946198739</v>
+      </c>
+      <c r="H46" s="14">
+        <f>G46+(G46*H$59)</f>
+        <v>85.234890039616275</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" s="14">
-        <f>(B34+B34*0.35%)</f>
-        <v>3.8634750000000002</v>
-      </c>
-      <c r="C41" s="14">
-        <f>(B41*2.12%)+B41</f>
-        <v>3.94538067</v>
-      </c>
-      <c r="D41" s="14">
-        <f>(C41*1.16%)+C41</f>
-        <v>3.9911470857719999</v>
-      </c>
-      <c r="E41" s="14">
-        <f>(D41*2.31%)+D41</f>
-        <v>4.0833425834533328</v>
-      </c>
-      <c r="F41" s="14">
-        <f>(E41*B52)+E41</f>
-        <v>4.1282593518713195</v>
-      </c>
-      <c r="G41" s="14">
-        <f>F41+(F41*B53)</f>
-        <v>4.2190810576124882</v>
-      </c>
-      <c r="H41" s="14">
-        <f>G41+(G41*B54)</f>
-        <v>4.4215969483778874</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>51</v>
-      </c>
-      <c r="G42" s="14">
-        <f>B32+(B32*G$57)</f>
-        <v>33.725999999999999</v>
-      </c>
-      <c r="H42" s="14">
-        <f>G42+(G42*H$57)</f>
-        <v>35.344847999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>53</v>
-      </c>
-      <c r="G43" s="14">
-        <f>B33+(B33*G$57)</f>
-        <v>3.4952399999999999</v>
-      </c>
-      <c r="H43" s="14">
-        <f>G43+(G43*H$57)</f>
-        <v>3.66301152</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>66</v>
-      </c>
-      <c r="G44" s="14">
-        <f>B35+(B35*G$57)</f>
-        <v>81.331001946198739</v>
-      </c>
-      <c r="H44" s="14">
-        <f>G44+(G44*H$57)</f>
-        <v>85.234890039616275</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="C47" s="18" t="s">
         <v>62</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>2015</v>
-      </c>
-      <c r="B47" s="40">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="C47" s="19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>2016</v>
-      </c>
-      <c r="B48" s="40">
-        <v>2.4E-2</v>
-      </c>
-      <c r="C48">
-        <v>100.66</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="B49" s="40">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="C49">
-        <v>103.361</v>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C49" s="19">
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="B50" s="40">
-        <v>2.3E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="C50">
-        <v>105.992</v>
+        <v>100.66</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="B51" s="40">
-        <v>2.8000000000000001E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="C51">
-        <v>107.819</v>
+        <v>103.361</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="B52" s="40">
-        <v>1.0999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="C52">
-        <v>108.736</v>
-      </c>
-      <c r="F52" s="15"/>
+        <v>105.992</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="B53" s="40">
-        <v>2.1999999999999999E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="C53">
-        <v>111.551</v>
-      </c>
-      <c r="F53" s="39"/>
+        <v>107.819</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="B54" s="40">
-        <v>4.8000000000000001E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="C54">
-        <v>121.664</v>
-      </c>
+        <v>108.736</v>
+      </c>
+      <c r="F54" s="15"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="A55">
+        <v>2021</v>
+      </c>
+      <c r="B55" s="40">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C55">
+        <v>111.551</v>
+      </c>
+      <c r="F55" s="39"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
+        <v>2022</v>
+      </c>
+      <c r="B56" s="40">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="C56">
+        <v>121.664</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>2015</v>
       </c>
-      <c r="B56">
+      <c r="B58">
         <v>2016</v>
       </c>
-      <c r="C56">
+      <c r="C58">
         <v>2017</v>
       </c>
-      <c r="D56">
+      <c r="D58">
         <v>2018</v>
       </c>
-      <c r="E56">
+      <c r="E58">
         <v>2019</v>
       </c>
-      <c r="F56">
+      <c r="F58">
         <v>2020</v>
       </c>
-      <c r="G56">
+      <c r="G58">
         <v>2021</v>
       </c>
-      <c r="H56">
+      <c r="H58">
         <v>2022</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="15">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="15">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B59" s="15">
         <v>2.4E-2</v>
       </c>
-      <c r="C57" s="15">
+      <c r="C59" s="15">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="D57" s="15">
+      <c r="D59" s="15">
         <v>2.3E-2</v>
       </c>
-      <c r="E57" s="15">
+      <c r="E59" s="15">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F57" s="15">
+      <c r="F59" s="15">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G57" s="15">
+      <c r="G59" s="15">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="H57" s="15">
+      <c r="H59" s="15">
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
@@ -3191,8 +3285,8 @@
   <hyperlinks>
     <hyperlink ref="M1" r:id="rId1" xr:uid="{8D5F4CF5-19E7-4407-B07A-CA114E2AF7CA}"/>
     <hyperlink ref="M2" r:id="rId2" location=":~:text=All%20relevant%20activity%20should%20now,no%20longer%20collect%20reference%20costs." xr:uid="{88339E28-F03E-4278-A978-A5848EF5A102}"/>
-    <hyperlink ref="M20" r:id="rId3" location="heading-2" xr:uid="{94C9397E-1A65-4633-A5A6-7EF3542DC68D}"/>
-    <hyperlink ref="C45" r:id="rId4" location=":~:text=The%20CPI%20inflation%20rate%20in,serious%20cost%20of%20living%20crisis." xr:uid="{0B43EB4C-AE01-46A8-A378-FC7EEBC4943D}"/>
+    <hyperlink ref="M21" r:id="rId3" location="heading-2" xr:uid="{94C9397E-1A65-4633-A5A6-7EF3542DC68D}"/>
+    <hyperlink ref="C47" r:id="rId4" location=":~:text=The%20CPI%20inflation%20rate%20in,serious%20cost%20of%20living%20crisis." xr:uid="{0B43EB4C-AE01-46A8-A378-FC7EEBC4943D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -3217,88 +3311,88 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="E2" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="45" t="s">
+    </row>
+    <row r="3" spans="1:19" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="O3" t="s">
+        <v>190</v>
+      </c>
+      <c r="P3" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>187</v>
+      </c>
+      <c r="R3" t="s">
+        <v>188</v>
+      </c>
+      <c r="S3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="42" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="B4" s="42">
+        <v>1517.223</v>
+      </c>
+      <c r="C4" s="42">
+        <v>1729.0409999999999</v>
+      </c>
+      <c r="D4" s="42">
+        <v>0.88</v>
+      </c>
+      <c r="E4" s="42">
+        <v>0.38</v>
+      </c>
+      <c r="F4" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="O3" t="s">
-        <v>192</v>
-      </c>
-      <c r="P3" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>189</v>
-      </c>
-      <c r="R3" t="s">
-        <v>190</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="G4" s="48"/>
+      <c r="H4" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="J4" s="50">
+        <v>2348.7959999999998</v>
+      </c>
+      <c r="K4" s="50">
+        <v>305.06760000000003</v>
+      </c>
+      <c r="L4" s="50">
+        <v>7.7</v>
+      </c>
+      <c r="N4" s="48" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="43">
-        <v>1517.223</v>
-      </c>
-      <c r="C4" s="43">
-        <v>1729.0409999999999</v>
-      </c>
-      <c r="D4" s="43">
-        <v>0.88</v>
-      </c>
-      <c r="E4" s="43">
-        <v>0.38</v>
-      </c>
-      <c r="F4" s="43" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="49"/>
-      <c r="H4" s="50" t="s">
-        <v>176</v>
-      </c>
-      <c r="J4" s="51">
-        <v>2348.7959999999998</v>
-      </c>
-      <c r="K4" s="51">
-        <v>305.06760000000003</v>
-      </c>
-      <c r="L4" s="51">
-        <v>7.7</v>
-      </c>
-      <c r="N4" s="49" t="s">
-        <v>193</v>
       </c>
       <c r="O4">
         <f>J4+J8+J16</f>
@@ -3322,39 +3416,39 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="43">
+      <c r="A5" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="42">
         <v>1217.4380000000001</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="42">
         <v>415.9633</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="42">
         <v>2.93</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="42">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F5" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="52" t="s">
-        <v>179</v>
-      </c>
-      <c r="J5" s="53" t="s">
-        <v>169</v>
-      </c>
-      <c r="K5" s="53">
+      <c r="F5" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="48"/>
+      <c r="H5" s="51" t="s">
+        <v>177</v>
+      </c>
+      <c r="J5" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="K5" s="52">
         <v>97.19538</v>
       </c>
-      <c r="L5" s="53" t="s">
-        <v>170</v>
-      </c>
-      <c r="N5" s="53" t="s">
-        <v>194</v>
+      <c r="L5" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="N5" s="52" t="s">
+        <v>192</v>
       </c>
       <c r="O5">
         <f>J4+J8+J16+J13</f>
@@ -3362,810 +3456,810 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="42">
+        <v>1676.0509999999999</v>
+      </c>
+      <c r="C6" s="42">
+        <v>385.98309999999998</v>
+      </c>
+      <c r="D6" s="42">
+        <v>4.34</v>
+      </c>
+      <c r="E6" s="42">
+        <v>0</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="48"/>
+      <c r="H6" s="51" t="s">
+        <v>178</v>
+      </c>
+      <c r="J6" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="K6" s="52">
+        <v>122.4042</v>
+      </c>
+      <c r="L6" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="N6" s="52" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="43">
+      <c r="B7" s="42">
+        <v>3956.6669999999999</v>
+      </c>
+      <c r="C7" s="42">
+        <v>829.37509999999997</v>
+      </c>
+      <c r="D7" s="42">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="E7" s="42">
+        <v>0</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="48"/>
+      <c r="H7" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="N7" s="48"/>
+    </row>
+    <row r="8" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="42">
+        <v>1967.914</v>
+      </c>
+      <c r="C8" s="42">
+        <v>311.49400000000003</v>
+      </c>
+      <c r="D8" s="42">
+        <v>6.32</v>
+      </c>
+      <c r="E8" s="42">
+        <v>0</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="48"/>
+      <c r="H8" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="J8" s="52">
+        <v>36.856340000000003</v>
+      </c>
+      <c r="K8" s="52">
+        <v>193.84370000000001</v>
+      </c>
+      <c r="L8" s="52">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="51" t="s">
+        <v>150</v>
+      </c>
+      <c r="J9" s="52">
+        <v>62.707299999999996</v>
+      </c>
+      <c r="K9" s="52">
+        <v>177.3931</v>
+      </c>
+      <c r="L9" s="52">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="42">
+        <v>251.7046</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="42">
+        <v>0</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="48"/>
+      <c r="H10" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="J10" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="K10" s="52">
+        <v>182.52770000000001</v>
+      </c>
+      <c r="L10" s="52" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="42">
+        <v>233.99279999999999</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="42">
+        <v>0</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" s="48"/>
+      <c r="H11" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="J11" s="52">
+        <v>59.025919999999999</v>
+      </c>
+      <c r="K11" s="52">
+        <v>226.9982</v>
+      </c>
+      <c r="L11" s="52">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+    </row>
+    <row r="13" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="42">
+        <v>343.80869999999999</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="42">
+        <v>0</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="48"/>
+      <c r="H13" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13" s="52">
+        <v>-921.35360000000003</v>
+      </c>
+      <c r="K13" s="52">
+        <v>251.7046</v>
+      </c>
+      <c r="L13" s="52" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="42">
+        <v>319.97449999999998</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="42">
+        <v>0</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="48"/>
+      <c r="H14" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="J14" s="52">
+        <v>-1514.1890000000001</v>
+      </c>
+      <c r="K14" s="52">
+        <v>233.99279999999999</v>
+      </c>
+      <c r="L14" s="52" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="42">
+        <v>5406.9380000000001</v>
+      </c>
+      <c r="C15" s="42">
+        <v>1400.335</v>
+      </c>
+      <c r="D15" s="42">
+        <v>3.86</v>
+      </c>
+      <c r="E15" s="42">
+        <v>0</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="H15" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="I15" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="J15" s="52">
+        <v>5406.9380000000001</v>
+      </c>
+      <c r="K15" s="52">
+        <v>1400.335</v>
+      </c>
+      <c r="L15" s="52">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="42">
+        <v>2269.1379999999999</v>
+      </c>
+      <c r="C16" s="42">
+        <v>806.8528</v>
+      </c>
+      <c r="D16" s="42">
+        <v>2.81</v>
+      </c>
+      <c r="E16" s="42">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F16" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="48" t="s">
+        <v>184</v>
+      </c>
+      <c r="J16" s="52">
+        <v>1217.4380000000001</v>
+      </c>
+      <c r="K16" s="52">
+        <v>415.9633</v>
+      </c>
+      <c r="L16" s="52">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="42">
+        <v>91.535179999999997</v>
+      </c>
+      <c r="C17" s="42">
+        <v>91.503929999999997</v>
+      </c>
+      <c r="D17" s="42">
+        <v>1</v>
+      </c>
+      <c r="E17" s="42">
+        <v>0.317</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="H17" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="J17" s="52">
         <v>1676.0509999999999</v>
       </c>
-      <c r="C6" s="43">
+      <c r="K17" s="52">
         <v>385.98309999999998</v>
       </c>
-      <c r="D6" s="43">
+      <c r="L17" s="52">
         <v>4.34</v>
       </c>
-      <c r="E6" s="43">
-        <v>0</v>
-      </c>
-      <c r="F6" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" s="49"/>
-      <c r="H6" s="52" t="s">
-        <v>180</v>
-      </c>
-      <c r="J6" s="53" t="s">
-        <v>173</v>
-      </c>
-      <c r="K6" s="53">
-        <v>122.4042</v>
-      </c>
-      <c r="L6" s="53" t="s">
-        <v>174</v>
-      </c>
-      <c r="N6" s="53" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="43">
+    </row>
+    <row r="18" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="42">
+        <v>162.3912</v>
+      </c>
+      <c r="C18" s="42">
+        <v>104.348</v>
+      </c>
+      <c r="D18" s="42">
+        <v>1.56</v>
+      </c>
+      <c r="E18" s="42">
+        <v>0.12</v>
+      </c>
+      <c r="F18" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="J18" s="52">
         <v>3956.6669999999999</v>
       </c>
-      <c r="C7" s="43">
+      <c r="K18" s="52">
         <v>829.37509999999997</v>
       </c>
-      <c r="D7" s="43">
+      <c r="L18" s="52">
         <v>4.7699999999999996</v>
       </c>
-      <c r="E7" s="43">
-        <v>0</v>
-      </c>
-      <c r="F7" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" s="49"/>
-      <c r="H7" s="53" t="s">
-        <v>181</v>
-      </c>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="N7" s="49"/>
-    </row>
-    <row r="8" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" s="43">
-        <v>1967.914</v>
-      </c>
-      <c r="C8" s="43">
-        <v>311.49400000000003</v>
-      </c>
-      <c r="D8" s="43">
-        <v>6.32</v>
-      </c>
-      <c r="E8" s="43">
-        <v>0</v>
-      </c>
-      <c r="F8" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="G8" s="49"/>
-      <c r="H8" s="52" t="s">
-        <v>150</v>
-      </c>
-      <c r="J8" s="53">
-        <v>36.856340000000003</v>
-      </c>
-      <c r="K8" s="53">
-        <v>193.84370000000001</v>
-      </c>
-      <c r="L8" s="53">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="J9" s="53">
-        <v>62.707299999999996</v>
-      </c>
-      <c r="K9" s="53">
-        <v>177.3931</v>
-      </c>
-      <c r="L9" s="53">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="B10" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10" s="43">
-        <v>251.7046</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" s="43">
-        <v>0</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="G10" s="49"/>
-      <c r="H10" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="J10" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="K10" s="53">
-        <v>182.52770000000001</v>
-      </c>
-      <c r="L10" s="53" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="43">
-        <v>233.99279999999999</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" s="43">
-        <v>0</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="G11" s="49"/>
-      <c r="H11" s="52" t="s">
-        <v>158</v>
-      </c>
-      <c r="J11" s="53">
-        <v>59.025919999999999</v>
-      </c>
-      <c r="K11" s="53">
-        <v>226.9982</v>
-      </c>
-      <c r="L11" s="53">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="54" t="s">
-        <v>104</v>
-      </c>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-    </row>
-    <row r="13" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="43">
-        <v>343.80869999999999</v>
-      </c>
-      <c r="D13" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" s="43">
-        <v>0</v>
-      </c>
-      <c r="F13" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="G13" s="49"/>
-      <c r="H13" s="52" t="s">
-        <v>105</v>
-      </c>
-      <c r="J13" s="53">
-        <v>-921.35360000000003</v>
-      </c>
-      <c r="K13" s="53">
-        <v>251.7046</v>
-      </c>
-      <c r="L13" s="53" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="B14" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="C14" s="43">
-        <v>319.97449999999998</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="E14" s="43">
-        <v>0</v>
-      </c>
-      <c r="F14" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="G14" s="49"/>
-      <c r="H14" s="52" t="s">
-        <v>109</v>
-      </c>
-      <c r="J14" s="53">
-        <v>-1514.1890000000001</v>
-      </c>
-      <c r="K14" s="53">
-        <v>233.99279999999999</v>
-      </c>
-      <c r="L14" s="53" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" s="43">
-        <v>5406.9380000000001</v>
-      </c>
-      <c r="C15" s="43">
-        <v>1400.335</v>
-      </c>
-      <c r="D15" s="43">
-        <v>3.86</v>
-      </c>
-      <c r="E15" s="43">
-        <v>0</v>
-      </c>
-      <c r="F15" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="H15" s="52" t="s">
-        <v>122</v>
-      </c>
-      <c r="I15" s="49" t="s">
+    </row>
+    <row r="19" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="42">
+        <v>147.03579999999999</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="42">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="H19" s="51" t="s">
+        <v>185</v>
+      </c>
+      <c r="I19" s="52" t="s">
         <v>182</v>
       </c>
-      <c r="J15" s="53">
-        <v>5406.9380000000001</v>
-      </c>
-      <c r="K15" s="53">
-        <v>1400.335</v>
-      </c>
-      <c r="L15" s="53">
-        <v>3.86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" s="43">
-        <v>2269.1379999999999</v>
-      </c>
-      <c r="C16" s="43">
-        <v>806.8528</v>
-      </c>
-      <c r="D16" s="43">
-        <v>2.81</v>
-      </c>
-      <c r="E16" s="43">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F16" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="H16" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="I16" s="49" t="s">
-        <v>186</v>
-      </c>
-      <c r="J16" s="53">
-        <v>1217.4380000000001</v>
-      </c>
-      <c r="K16" s="53">
-        <v>415.9633</v>
-      </c>
-      <c r="L16" s="53">
-        <v>2.93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="B17" s="43">
-        <v>91.535179999999997</v>
-      </c>
-      <c r="C17" s="43">
-        <v>91.503929999999997</v>
-      </c>
-      <c r="D17" s="43">
-        <v>1</v>
-      </c>
-      <c r="E17" s="43">
-        <v>0.317</v>
-      </c>
-      <c r="F17" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="H17" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="I17" s="49" t="s">
-        <v>185</v>
-      </c>
-      <c r="J17" s="53">
-        <v>1676.0509999999999</v>
-      </c>
-      <c r="K17" s="53">
-        <v>385.98309999999998</v>
-      </c>
-      <c r="L17" s="53">
-        <v>4.34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="43">
-        <v>162.3912</v>
-      </c>
-      <c r="C18" s="43">
-        <v>104.348</v>
-      </c>
-      <c r="D18" s="43">
-        <v>1.56</v>
-      </c>
-      <c r="E18" s="43">
-        <v>0.12</v>
-      </c>
-      <c r="F18" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="H18" s="52" t="s">
-        <v>100</v>
-      </c>
-      <c r="I18" s="49" t="s">
-        <v>183</v>
-      </c>
-      <c r="J18" s="53">
-        <v>3956.6669999999999</v>
-      </c>
-      <c r="K18" s="53">
-        <v>829.37509999999997</v>
-      </c>
-      <c r="L18" s="53">
-        <v>4.7699999999999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="B19" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="C19" s="43">
-        <v>147.03579999999999</v>
-      </c>
-      <c r="D19" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="E19" s="43">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="F19" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="H19" s="52" t="s">
-        <v>187</v>
-      </c>
-      <c r="I19" s="53" t="s">
-        <v>184</v>
-      </c>
-      <c r="J19" s="49">
+      <c r="J19" s="48">
         <f>AVERAGE(J16:J17)</f>
         <v>1446.7445</v>
       </c>
-      <c r="K19" s="49">
+      <c r="K19" s="48">
         <f>AVERAGE(K16:K17)</f>
         <v>400.97320000000002</v>
       </c>
-      <c r="L19" s="49">
+      <c r="L19" s="48">
         <f>AVERAGE(L16:L17)</f>
         <v>3.6349999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="42">
+        <v>90.557829999999996</v>
+      </c>
+      <c r="D20" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="E20" s="42">
+        <v>0.255</v>
+      </c>
+      <c r="F20" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="C20" s="43">
-        <v>90.557829999999996</v>
-      </c>
-      <c r="D20" s="43" t="s">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="43">
-        <v>0.255</v>
-      </c>
-      <c r="F20" s="43" t="s">
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+    </row>
+    <row r="22" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
+      <c r="B22" s="42">
+        <v>190.4007</v>
+      </c>
+      <c r="C22" s="42">
+        <v>173.78120000000001</v>
+      </c>
+      <c r="D22" s="42">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E22" s="42">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="F22" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-    </row>
-    <row r="22" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
+    </row>
+    <row r="23" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="B22" s="43">
-        <v>190.4007</v>
-      </c>
-      <c r="C22" s="43">
-        <v>173.78120000000001</v>
-      </c>
-      <c r="D22" s="43">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E22" s="43">
-        <v>0.27300000000000002</v>
-      </c>
-      <c r="F22" s="43" t="s">
+      <c r="B23" s="42">
+        <v>171.73500000000001</v>
+      </c>
+      <c r="C23" s="42">
+        <v>300.59230000000002</v>
+      </c>
+      <c r="D23" s="42">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E23" s="42">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="F23" s="42" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="B23" s="43">
-        <v>171.73500000000001</v>
-      </c>
-      <c r="C23" s="43">
-        <v>300.59230000000002</v>
-      </c>
-      <c r="D23" s="43">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="E23" s="43">
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="F23" s="43" t="s">
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="42" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="48" t="s">
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+    </row>
+    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-    </row>
-    <row r="25" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
+      <c r="B26" s="42">
+        <v>153.2397</v>
+      </c>
+      <c r="C26" s="42">
+        <v>242.29499999999999</v>
+      </c>
+      <c r="D26" s="42">
+        <v>0.63</v>
+      </c>
+      <c r="E26" s="42">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="F26" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-    </row>
-    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
+    </row>
+    <row r="27" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="B26" s="43">
-        <v>153.2397</v>
-      </c>
-      <c r="C26" s="43">
-        <v>242.29499999999999</v>
-      </c>
-      <c r="D26" s="43">
-        <v>0.63</v>
-      </c>
-      <c r="E26" s="43">
-        <v>0.52700000000000002</v>
-      </c>
-      <c r="F26" s="43" t="s">
+      <c r="B27" s="42">
+        <v>390.0575</v>
+      </c>
+      <c r="C27" s="42">
+        <v>387.77379999999999</v>
+      </c>
+      <c r="D27" s="42">
+        <v>1.01</v>
+      </c>
+      <c r="E27" s="42">
+        <v>0.314</v>
+      </c>
+      <c r="F27" s="42" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="B27" s="43">
-        <v>390.0575</v>
-      </c>
-      <c r="C27" s="43">
-        <v>387.77379999999999</v>
-      </c>
-      <c r="D27" s="43">
-        <v>1.01</v>
-      </c>
-      <c r="E27" s="43">
-        <v>0.314</v>
-      </c>
-      <c r="F27" s="43" t="s">
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+    </row>
+    <row r="29" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="42" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="s">
+      <c r="B29" s="42">
+        <v>36.856340000000003</v>
+      </c>
+      <c r="C29" s="42">
+        <v>193.84370000000001</v>
+      </c>
+      <c r="D29" s="42">
+        <v>0.19</v>
+      </c>
+      <c r="E29" s="42">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="F29" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-    </row>
-    <row r="29" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="43" t="s">
+    </row>
+    <row r="30" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="B29" s="43">
-        <v>36.856340000000003</v>
-      </c>
-      <c r="C29" s="43">
-        <v>193.84370000000001</v>
-      </c>
-      <c r="D29" s="43">
-        <v>0.19</v>
-      </c>
-      <c r="E29" s="43">
-        <v>0.84899999999999998</v>
-      </c>
-      <c r="F29" s="43" t="s">
+      <c r="B30" s="42">
+        <v>62.707299999999996</v>
+      </c>
+      <c r="C30" s="42">
+        <v>177.3931</v>
+      </c>
+      <c r="D30" s="42">
+        <v>0.35</v>
+      </c>
+      <c r="E30" s="42">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="F30" s="42" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="43" t="s">
+    <row r="31" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="B30" s="43">
-        <v>62.707299999999996</v>
-      </c>
-      <c r="C30" s="43">
-        <v>177.3931</v>
-      </c>
-      <c r="D30" s="43">
-        <v>0.35</v>
-      </c>
-      <c r="E30" s="43">
-        <v>0.72399999999999998</v>
-      </c>
-      <c r="F30" s="43" t="s">
+      <c r="B31" s="42" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="43" t="s">
+      <c r="C31" s="42">
+        <v>182.52770000000001</v>
+      </c>
+      <c r="D31" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="E31" s="42">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="F31" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="C31" s="43">
-        <v>182.52770000000001</v>
-      </c>
-      <c r="D31" s="43" t="s">
+    </row>
+    <row r="32" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="E31" s="43">
-        <v>0.66500000000000004</v>
-      </c>
-      <c r="F31" s="43" t="s">
+      <c r="B32" s="42">
+        <v>59.025919999999999</v>
+      </c>
+      <c r="C32" s="42">
+        <v>226.9982</v>
+      </c>
+      <c r="D32" s="42">
+        <v>0.26</v>
+      </c>
+      <c r="E32" s="42">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="F32" s="42" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="43" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="41" t="s">
         <v>158</v>
       </c>
-      <c r="B32" s="43">
-        <v>59.025919999999999</v>
-      </c>
-      <c r="C32" s="43">
-        <v>226.9982</v>
-      </c>
-      <c r="D32" s="43">
-        <v>0.26</v>
-      </c>
-      <c r="E32" s="43">
-        <v>0.79500000000000004</v>
-      </c>
-      <c r="F32" s="43" t="s">
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+    </row>
+    <row r="34" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="42" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="42" t="s">
+      <c r="B34" s="42">
+        <v>207.67949999999999</v>
+      </c>
+      <c r="C34" s="42">
+        <v>95.780289999999994</v>
+      </c>
+      <c r="D34" s="42">
+        <v>2.17</v>
+      </c>
+      <c r="E34" s="42">
+        <v>0.03</v>
+      </c>
+      <c r="F34" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-    </row>
-    <row r="34" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="43" t="s">
+    </row>
+    <row r="35" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="B34" s="43">
-        <v>207.67949999999999</v>
-      </c>
-      <c r="C34" s="43">
-        <v>95.780289999999994</v>
-      </c>
-      <c r="D34" s="43">
-        <v>2.17</v>
-      </c>
-      <c r="E34" s="43">
-        <v>0.03</v>
-      </c>
-      <c r="F34" s="43" t="s">
+      <c r="B35" s="42">
+        <v>258.07220000000001</v>
+      </c>
+      <c r="C35" s="42">
+        <v>113.32259999999999</v>
+      </c>
+      <c r="D35" s="42">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="E35" s="42">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F35" s="42" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="43" t="s">
+    <row r="36" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="B35" s="43">
-        <v>258.07220000000001</v>
-      </c>
-      <c r="C35" s="43">
-        <v>113.32259999999999</v>
-      </c>
-      <c r="D35" s="43">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="E35" s="43">
-        <v>2.3E-2</v>
-      </c>
-      <c r="F35" s="43" t="s">
+      <c r="B36" s="42">
+        <v>1257.9680000000001</v>
+      </c>
+      <c r="C36" s="42">
+        <v>623.30529999999999</v>
+      </c>
+      <c r="D36" s="42">
+        <v>2.02</v>
+      </c>
+      <c r="E36" s="42">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F36" s="42" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="43" t="s">
+    <row r="37" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="41" t="s">
         <v>165</v>
       </c>
-      <c r="B36" s="43">
-        <v>1257.9680000000001</v>
-      </c>
-      <c r="C36" s="43">
-        <v>623.30529999999999</v>
-      </c>
-      <c r="D36" s="43">
-        <v>2.02</v>
-      </c>
-      <c r="E36" s="43">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="F36" s="43" t="s">
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+    </row>
+    <row r="38" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="42" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="42" t="s">
+      <c r="B38" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-    </row>
-    <row r="38" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="43" t="s">
+      <c r="C38" s="42">
+        <v>97.19538</v>
+      </c>
+      <c r="D38" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="E38" s="42">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="F38" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="C38" s="43">
-        <v>97.19538</v>
-      </c>
-      <c r="D38" s="43" t="s">
+    </row>
+    <row r="39" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="42" t="s">
         <v>170</v>
       </c>
-      <c r="E38" s="43">
-        <v>0.55600000000000005</v>
-      </c>
-      <c r="F38" s="43" t="s">
+      <c r="B39" s="42" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="43" t="s">
+      <c r="C39" s="42">
+        <v>122.4042</v>
+      </c>
+      <c r="D39" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="B39" s="43" t="s">
+      <c r="E39" s="42">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F39" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="C39" s="43">
-        <v>122.4042</v>
-      </c>
-      <c r="D39" s="43" t="s">
+    </row>
+    <row r="40" spans="1:6" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="E39" s="43">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="F39" s="43" t="s">
+      <c r="B40" s="45">
+        <v>2348.7959999999998</v>
+      </c>
+      <c r="C40" s="45">
+        <v>305.06760000000003</v>
+      </c>
+      <c r="D40" s="45">
+        <v>7.7</v>
+      </c>
+      <c r="E40" s="45">
+        <v>0</v>
+      </c>
+      <c r="F40" s="45" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="B40" s="46">
-        <v>2348.7959999999998</v>
-      </c>
-      <c r="C40" s="46">
-        <v>305.06760000000003</v>
-      </c>
-      <c r="D40" s="46">
-        <v>7.7</v>
-      </c>
-      <c r="E40" s="46">
-        <v>0</v>
-      </c>
-      <c r="F40" s="46" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -4178,8 +4272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE0144D-358F-44D8-95C5-63A01C199E30}">
   <dimension ref="B1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4191,36 +4285,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="39" x14ac:dyDescent="0.25">
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="54" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="54" t="s">
         <v>203</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="G1" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="F1" s="55" t="s">
-        <v>205</v>
-      </c>
-      <c r="G1" s="56" t="s">
-        <v>206</v>
-      </c>
-      <c r="H1" s="56"/>
-      <c r="I1" s="57" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="58"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D2">
         <v>7.4516567327989689</v>
       </c>
       <c r="E2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -4239,21 +4333,21 @@
         <v>8.1968224060788675</v>
       </c>
       <c r="K2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D3">
         <v>1.0856698902187309</v>
       </c>
       <c r="E3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -4272,21 +4366,21 @@
         <v>1.1942368792406022</v>
       </c>
       <c r="K3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D4">
         <v>10.230186979795642</v>
       </c>
       <c r="E4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -4305,41 +4399,41 @@
         <v>11.253205677775204</v>
       </c>
       <c r="K4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="39" x14ac:dyDescent="0.25">
-      <c r="B7" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="55" t="s">
+      <c r="B7" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>202</v>
+      </c>
+      <c r="F7" s="54" t="s">
         <v>203</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="G7" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="F7" s="55" t="s">
-        <v>205</v>
-      </c>
-      <c r="G7" s="56" t="s">
-        <v>206</v>
-      </c>
-      <c r="H7" s="56"/>
-      <c r="I7" s="57" t="s">
-        <v>92</v>
-      </c>
-      <c r="J7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="58"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D8">
-        <f>D2+D2*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <f>D2+D2*('diagnostic costs'!$C$56-'diagnostic costs'!$C$51)/'diagnostic costs'!$C$56</f>
         <v>8.5726758771672245</v>
       </c>
       <c r="E8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -4352,24 +4446,24 @@
         <v>8.572675877167224E-2</v>
       </c>
       <c r="I8">
-        <f>I2+I2*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <f>I2+I2*('diagnostic costs'!$C$56-'diagnostic costs'!$C$51)/'diagnostic costs'!$C$56</f>
         <v>7.7154082894505009</v>
       </c>
       <c r="J8">
-        <f>J2+J2*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <f>J2+J2*('diagnostic costs'!$C$56-'diagnostic costs'!$C$51)/'diagnostic costs'!$C$56</f>
         <v>9.4299434648839497</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D9">
-        <f>D3+D3*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <f>D3+D3*('diagnostic costs'!$C$56-'diagnostic costs'!$C$51)/'diagnostic costs'!$C$56</f>
         <v>1.2489968891721883</v>
       </c>
       <c r="E9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -4382,24 +4476,24 @@
         <v>1.2489968891721883E-2</v>
       </c>
       <c r="I9">
-        <f>I3+I3*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <f>I3+I3*('diagnostic costs'!$C$56-'diagnostic costs'!$C$51)/'diagnostic costs'!$C$56</f>
         <v>1.1240972002549696</v>
       </c>
       <c r="J9">
-        <f>J3+J3*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <f>J3+J3*('diagnostic costs'!$C$56-'diagnostic costs'!$C$51)/'diagnostic costs'!$C$56</f>
         <v>1.373896578089405</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D10">
-        <f>D4+D4*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <f>D4+D4*('diagnostic costs'!$C$56-'diagnostic costs'!$C$51)/'diagnostic costs'!$C$56</f>
         <v>11.769205196286959</v>
       </c>
       <c r="E10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -4412,17 +4506,17 @@
         <v>0.1176920519628696</v>
       </c>
       <c r="I10">
-        <f>I4+I4*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <f>I4+I4*('diagnostic costs'!$C$56-'diagnostic costs'!$C$51)/'diagnostic costs'!$C$56</f>
         <v>10.592284676658261</v>
       </c>
       <c r="J10">
-        <f>J4+J4*('diagnostic costs'!$C$54-'diagnostic costs'!$C$49)/'diagnostic costs'!$C$54</f>
+        <f>J4+J4*('diagnostic costs'!$C$56-'diagnostic costs'!$C$51)/'diagnostic costs'!$C$56</f>
         <v>12.946125715915652</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>